<commit_message>
more tables and updated UML
</commit_message>
<xml_diff>
--- a/tabelas MR.xlsx
+++ b/tabelas MR.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="6135" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="6135" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Pessoa" sheetId="2" r:id="rId2"/>
-    <sheet name="UrgenciaMedica" sheetId="5" r:id="rId3"/>
+    <sheet name="a" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="82">
   <si>
     <t>Pessoa</t>
   </si>
@@ -142,15 +142,6 @@
     <t>Atributos mais acedidos: nome</t>
   </si>
   <si>
-    <t>Funcionario</t>
-  </si>
-  <si>
-    <t>Chave candidata: numeroUtente</t>
-  </si>
-  <si>
-    <t>Chave primaria: numeroUtente</t>
-  </si>
-  <si>
     <t>Especialidade</t>
   </si>
   <si>
@@ -199,9 +190,6 @@
     <t>Atributos mais acedidos: func-ID, area</t>
   </si>
   <si>
-    <t>Atributos mais acedidos: func-ID</t>
-  </si>
-  <si>
     <t>pessoa-ID</t>
   </si>
   <si>
@@ -235,12 +223,6 @@
     <t>Chave primária: alergia-ID</t>
   </si>
   <si>
-    <t>FALTA FAZER ASSOCIACAO * - * DOS FARMACOS E ALERGIAS</t>
-  </si>
-  <si>
-    <t>Atr. mais acedidos: numeroUtente</t>
-  </si>
-  <si>
     <t>Atr. mais acedidos: (numeroUtente) (farm-ID)</t>
   </si>
   <si>
@@ -263,6 +245,33 @@
   </si>
   <si>
     <t>Atr. mais acedidos: (numeroUtente) (alergia-ID)</t>
+  </si>
+  <si>
+    <t>Técnico</t>
+  </si>
+  <si>
+    <t>Chave candidata: (pessoa-ID) (func-ID)</t>
+  </si>
+  <si>
+    <t>Chave primaria: (pessoa-ID) (func-ID)</t>
+  </si>
+  <si>
+    <t>Atributos mais acedidos: (pessoa-ID) (func-ID)</t>
+  </si>
+  <si>
+    <t>Chave candidata: (pessoa-ID) (numeroUtente)</t>
+  </si>
+  <si>
+    <t>Chave primaria: (pessoa-ID) (numeroUtente)</t>
+  </si>
+  <si>
+    <t>Atr. mais acedidos: (pessoa-ID) (numeroUtente)</t>
+  </si>
+  <si>
+    <t>Chave primaria: pessoa-ID</t>
+  </si>
+  <si>
+    <t>Atributos mais acedidos: pessoa-ID</t>
   </si>
 </sst>
 </file>
@@ -767,8 +776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11:G18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -779,9 +788,9 @@
     <col min="5" max="5" width="19.85546875" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" customWidth="1"/>
     <col min="7" max="7" width="16.42578125" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" customWidth="1"/>
-    <col min="10" max="10" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" customWidth="1"/>
+    <col min="9" max="9" width="16" customWidth="1"/>
+    <col min="10" max="10" width="8.28515625" customWidth="1"/>
+    <col min="11" max="11" width="12.85546875" customWidth="1"/>
     <col min="13" max="13" width="15.140625" customWidth="1"/>
     <col min="14" max="14" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8.5703125" bestFit="1" customWidth="1"/>
@@ -805,7 +814,7 @@
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
       <c r="I1" s="3" t="s">
-        <v>38</v>
+        <v>2</v>
       </c>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
@@ -814,11 +823,6 @@
       </c>
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
-      <c r="Q1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
       <c r="U1" s="3" t="s">
         <v>3</v>
       </c>
@@ -862,15 +866,6 @@
       <c r="O3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="Q3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="U3" s="2" t="s">
         <v>24</v>
       </c>
@@ -883,7 +878,7 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
         <v>31</v>
@@ -892,7 +887,7 @@
         <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="F4" t="s">
         <v>31</v>
@@ -901,7 +896,7 @@
         <v>20</v>
       </c>
       <c r="I4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="J4" t="s">
         <v>31</v>
@@ -910,7 +905,7 @@
         <v>20</v>
       </c>
       <c r="M4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="N4" t="s">
         <v>31</v>
@@ -918,17 +913,8 @@
       <c r="O4" t="s">
         <v>20</v>
       </c>
-      <c r="Q4" t="s">
-        <v>53</v>
-      </c>
-      <c r="R4" t="s">
-        <v>31</v>
-      </c>
-      <c r="S4" t="s">
-        <v>20</v>
-      </c>
       <c r="U4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="V4" t="s">
         <v>31</v>
@@ -947,14 +933,32 @@
       <c r="C5" t="s">
         <v>33</v>
       </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K5" t="s">
+        <v>20</v>
+      </c>
       <c r="U5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="V5" t="s">
         <v>31</v>
       </c>
       <c r="W5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
@@ -967,17 +971,8 @@
       <c r="C6" t="s">
         <v>34</v>
       </c>
-      <c r="E6" t="s">
-        <v>39</v>
-      </c>
-      <c r="I6" t="s">
-        <v>54</v>
-      </c>
       <c r="M6" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
@@ -991,19 +986,16 @@
         <v>35</v>
       </c>
       <c r="E7" t="s">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="I7" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="M7" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="U7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
@@ -1017,47 +1009,78 @@
         <v>36</v>
       </c>
       <c r="E8" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="I8" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="M8" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="U8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>79</v>
+      </c>
+      <c r="I9" t="s">
+        <v>76</v>
+      </c>
       <c r="U9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>37</v>
       </c>
+      <c r="E12" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="I12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
       <c r="U12" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="V12" s="3"/>
       <c r="W12" s="3"/>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="E14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="U14" s="2" t="s">
         <v>24</v>
       </c>
@@ -1069,8 +1092,26 @@
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15" t="s">
+        <v>20</v>
+      </c>
+      <c r="I15" t="s">
+        <v>54</v>
+      </c>
+      <c r="J15" t="s">
+        <v>31</v>
+      </c>
+      <c r="K15" t="s">
+        <v>20</v>
+      </c>
       <c r="U15" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="V15" t="s">
         <v>31</v>
@@ -1081,42 +1122,60 @@
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="U16" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="V16" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="W16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="9:21" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>55</v>
+      </c>
+      <c r="I17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>80</v>
+      </c>
       <c r="I18" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="U18" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="19" spans="9:21" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>81</v>
+      </c>
+      <c r="I19" t="s">
+        <v>81</v>
+      </c>
       <c r="U19" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="9:21" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="5:21" x14ac:dyDescent="0.25">
       <c r="U20" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
     <mergeCell ref="U12:W12"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="I1:K1"/>
     <mergeCell ref="M1:O1"/>
-    <mergeCell ref="Q1:S1"/>
     <mergeCell ref="U1:W1"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="I12:K12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1126,7 +1185,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11:C11"/>
     </sheetView>
   </sheetViews>
@@ -1142,12 +1201,12 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="E1" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
@@ -1174,7 +1233,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
         <v>31</v>
@@ -1183,7 +1242,7 @@
         <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F4" t="s">
         <v>31</v>
@@ -1214,18 +1273,18 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E7" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E8" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1238,12 +1297,12 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="E11" s="3" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
@@ -1279,7 +1338,7 @@
         <v>20</v>
       </c>
       <c r="E13" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F13" t="s">
         <v>31</v>
@@ -1290,7 +1349,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B14" t="s">
         <v>31</v>
@@ -1299,7 +1358,7 @@
         <v>20</v>
       </c>
       <c r="E14" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F14" t="s">
         <v>31</v>
@@ -1310,26 +1369,26 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E16" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="E17" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E18" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>